<commit_message>
Atualição da planilha de dados após nova avaliação dos testes 12A e 13A
</commit_message>
<xml_diff>
--- a/assessment-data/Dados.xlsx
+++ b/assessment-data/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Mestrado\sample\assessment-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8227190-AFE8-4D05-A036-975BCE44B253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF00DB1-7D69-4197-8516-E81F37EC7382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9A545A00-4E6E-4670-843B-8A547C2EF924}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -811,7 +811,184 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="77">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -828,6 +1005,78 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
@@ -949,6 +1198,34 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1097,7 +1374,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="User" refreshedDate="45376.527854745371" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="30" xr:uid="{BB94BCED-0EED-4FA3-B768-059DA8E77F9C}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="User" refreshedDate="45376.90828541667" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="30" xr:uid="{BB94BCED-0EED-4FA3-B768-059DA8E77F9C}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N31" sheet="Avaliação por Tipo de Ref."/>
   </cacheSource>
@@ -1546,7 +1823,7 @@
     <s v="Vide commits"/>
     <s v="Vide commits"/>
     <s v="Not Changed Behavior"/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -1578,7 +1855,7 @@
     <s v="Vide commits"/>
     <s v="Vide commits"/>
     <s v="Not Changed Behavior"/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -1665,7 +1942,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F614FAE5-0CB0-47D9-8502-503333F55A20}" name="Tabela dinâmica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F614FAE5-0CB0-47D9-8502-503333F55A20}" name="Tabela dinâmica1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D5:G25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -1798,8 +2075,8 @@
   <dataFields count="1">
     <dataField name="Contagem de #" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="20">
-    <format dxfId="37">
+  <formats count="29">
+    <format dxfId="76">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -1814,7 +2091,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1822,6 +2099,276 @@
           </reference>
           <reference field="3" count="1">
             <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="5"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="70">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="68">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="5">
+            <x v="1"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="5">
+            <x v="1"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="66">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="2">
+            <x v="6"/>
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="2">
+            <x v="6"/>
+            <x v="10"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="2">
+            <x v="4"/>
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="59">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="2">
+            <x v="4"/>
+            <x v="9"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="10"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="57">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -1830,25 +2377,28 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
             <x v="1"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="34">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
           <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
             <x v="1"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -1860,223 +2410,71 @@
             <x v="2"/>
           </reference>
           <reference field="3" count="1">
-            <x v="2"/>
+            <x v="11"/>
           </reference>
           <reference field="12" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="2"/>
+            <x v="1"/>
           </reference>
           <reference field="3" count="1">
-            <x v="2"/>
-          </reference>
+            <x v="6"/>
+          </reference>
+          <reference field="12" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="11"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="5">
-            <x v="1"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="13"/>
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="5">
-            <x v="1"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="13"/>
-            <x v="14"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
             <x v="1"/>
           </reference>
           <reference field="3" count="1">
-            <x v="3"/>
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="3"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
             <x v="1"/>
           </reference>
-          <reference field="3" count="2">
+          <reference field="3" count="1">
             <x v="6"/>
-            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="2">
-            <x v="6"/>
-            <x v="10"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
-            <x v="2"/>
+            <x v="1"/>
           </reference>
           <reference field="3" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="21">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="2">
-            <x v="4"/>
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="20">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="2">
-            <x v="4"/>
-            <x v="9"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="1"/>
+            <x v="12"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="1">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="1">
-            <x v="10"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
             <x v="1"/>
           </reference>
           <reference field="3" count="1">
-            <x v="10"/>
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -2414,10 +2812,10 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="J17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N30" sqref="A29:N30"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3281,7 +3679,7 @@
         <v>56</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N24" s="9"/>
     </row>
@@ -3351,7 +3749,7 @@
         <v>56</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N26" s="9"/>
     </row>
@@ -3545,7 +3943,7 @@
   <dimension ref="D5:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3657,10 +4055,10 @@
         <v>23</v>
       </c>
       <c r="E13" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" s="22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G13" s="22">
         <v>10</v>
@@ -3679,14 +4077,12 @@
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="23">
-        <v>1</v>
-      </c>
-      <c r="F15" s="22">
-        <v>1</v>
+      <c r="E15" s="22"/>
+      <c r="F15" s="24">
+        <v>2</v>
       </c>
       <c r="G15" s="22">
         <v>2</v>
@@ -3719,14 +4115,12 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="23">
-        <v>1</v>
-      </c>
-      <c r="F18" s="22">
-        <v>1</v>
+      <c r="E18" s="22"/>
+      <c r="F18" s="24">
+        <v>2</v>
       </c>
       <c r="G18" s="22">
         <v>2</v>
@@ -3765,7 +4159,7 @@
       <c r="E21" s="23">
         <v>1</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="24">
         <v>1</v>
       </c>
       <c r="G21" s="22">
@@ -3803,7 +4197,7 @@
       <c r="E24" s="23">
         <v>1</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="24">
         <v>1</v>
       </c>
       <c r="G24" s="22">
@@ -3815,10 +4209,10 @@
         <v>38</v>
       </c>
       <c r="E25" s="22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F25" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G25" s="22">
         <v>30</v>

</xml_diff>